<commit_message>
Update schema files after changes to upstream_data_source
</commit_message>
<xml_diff>
--- a/project/excel/matrix_schema.xlsx
+++ b/project/excel/matrix_schema.xlsx
@@ -10,6 +10,7 @@
     <sheet name="MatrixNode" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="MatrixEdge" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="MatrixEdgeCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="MatrixNodeCollection" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -585,4 +586,30 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refresh generated schema files
</commit_message>
<xml_diff>
--- a/project/excel/matrix_schema.xlsx
+++ b/project/excel/matrix_schema.xlsx
@@ -11,6 +11,8 @@
     <sheet name="MatrixEdge" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="MatrixEdgeCollection" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="MatrixNodeCollection" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DiseaseListEntry" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MatrixDiseaseList" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -612,4 +614,286 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AU1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>category_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>definition</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>synonyms</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>subsets</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>crossreferences</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_matrix_manually_excluded</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_matrix_manually_included</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_clingen</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>is_grouping_subset</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>is_grouping_subset_ancestor</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>is_orphanet_subtype</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>is_orphanet_subtype_descendant</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>is_omimps</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>is_omimps_descendant</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>is_leaf</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>is_leaf_direct_parent</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>is_orphanet_disorder</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>is_omim</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>is_icd_category</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>is_icd_chapter_code</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>is_icd_chapter_header</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>is_icd_billable</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>is_mondo_subtype</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>is_pathway_defect</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>is_susceptibility</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>is_paraphilic</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>is_acquired</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>is_andor</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>is_withorwithout</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>is_obsoletion_candidate</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>is_unclassified_hereditary</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>official_matrix_filter</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>harrisons_view</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>mondo_txgnn</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>mondo_top_grouping</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>medical_specialization</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>txgnn</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>anatomical</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>is_pathogen_caused</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>is_cancer</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>is_glucose_dysfunction</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>tag_existing_treatment</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>tag_qaly_lost</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>subset_group_id</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>subset_group_label</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>other_subsets_count</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor model and presentation
</commit_message>
<xml_diff>
--- a/project/excel/matrix_schema.xlsx
+++ b/project/excel/matrix_schema.xlsx
@@ -581,7 +581,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>edges</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>nodes</t>
         </is>
       </c>
     </row>
@@ -889,7 +889,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>diseases_list_entries</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
programatically adds enumerations to the schema from biolink model
</commit_message>
<xml_diff>
--- a/project/excel/matrix_schema.xlsx
+++ b/project/excel/matrix_schema.xlsx
@@ -489,7 +489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,46 +520,59 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>agent_type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>primary_knowledge_source</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>aggregator_knowledge_source</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>publications</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>subject_aspect_qualifier</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>subject_direction_qualifier</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>object_aspect_qualifier</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>object_direction_qualifier</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>upstream_data_source</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"knowledge_assertion,logical_entailment,prediction,statistical_association,observation,not_provided"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"manual_agent,automated_agent,data_analysis_pipeline,computational_model,text_mining_agent,image_processing_agent,manual_validation_of_automated_agent,not_provided"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update hardcoded pandera schema to match schema definition from monorepo, also add num_sentences and num_references to the linkml schema and regenerate artifacts
</commit_message>
<xml_diff>
--- a/project/excel/matrix_schema.xlsx
+++ b/project/excel/matrix_schema.xlsx
@@ -489,7 +489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,16 @@
       <c r="M1" t="inlineStr">
         <is>
           <t>upstream_data_source</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>num_references</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>num_sentences</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add unified node and unified edge classes, update hand-made pandera schema
</commit_message>
<xml_diff>
--- a/project/excel/matrix_schema.xlsx
+++ b/project/excel/matrix_schema.xlsx
@@ -9,10 +9,12 @@
   <sheets>
     <sheet name="MatrixNode" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="MatrixEdge" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MatrixEdgeList" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MatrixNodeList" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="DiseaseListEntry" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="MatrixDiseaseList" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="UnionedNode" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="UnionedEdge" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MatrixEdgeList" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MatrixNodeList" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="DiseaseListEntry" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="MatrixDiseaseList" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -593,7 +595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,7 +606,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>edges</t>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>equivalent_identifiers</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>all_categories</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>publications</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>labels</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>international_resource_identifier</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>upstream_data_source</t>
         </is>
       </c>
     </row>
@@ -614,6 +661,115 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>primary_knowledge_sources</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>subject</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>predicate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>knowledge_level</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>agent_type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>primary_knowledge_source</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>aggregator_knowledge_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>publications</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subject_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subject_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>object_aspect_qualifier</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>object_direction_qualifier</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>upstream_data_source</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>num_references</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>num_sentences</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"knowledge_assertion,logical_entailment,prediction,statistical_association,observation,not_provided"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"manual_agent,automated_agent,data_analysis_pipeline,computational_model,text_mining_agent,image_processing_agent,manual_validation_of_automated_agent,not_provided"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -630,263 +786,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>nodes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AU1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>category_class</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>definition</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>synonyms</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>subsets</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>crossreferences</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>is_matrix_manually_excluded</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>is_matrix_manually_included</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_clingen</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>is_grouping_subset</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>is_grouping_subset_ancestor</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>is_orphanet_subtype</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>is_orphanet_subtype_descendant</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>is_omimps</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>is_omimps_descendant</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>is_leaf</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>is_leaf_direct_parent</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>is_orphanet_disorder</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>is_omim</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>is_icd_category</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>is_icd_chapter_code</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>is_icd_chapter_header</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>is_icd_billable</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>is_mondo_subtype</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>is_pathway_defect</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>is_susceptibility</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>is_paraphilic</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>is_acquired</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>is_andor</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>is_withorwithout</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>is_obsoletion_candidate</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>is_unclassified_hereditary</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>official_matrix_filter</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>harrisons_view</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>mondo_txgnn</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>mondo_top_grouping</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>medical_specialization</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>txgnn</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>anatomical</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>is_pathogen_caused</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>is_cancer</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>is_glucose_dysfunction</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>tag_existing_treatment</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>tag_qaly_lost</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>subset_group_id</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>subset_group_label</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>other_subsets_count</t>
+          <t>edges</t>
         </is>
       </c>
     </row>
@@ -912,6 +812,288 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>nodes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AU1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>category_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>definition</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>synonyms</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>subsets</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>crossreferences</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_matrix_manually_excluded</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_matrix_manually_included</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_clingen</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>is_grouping_subset</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>is_grouping_subset_ancestor</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>is_orphanet_subtype</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>is_orphanet_subtype_descendant</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>is_omimps</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>is_omimps_descendant</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>is_leaf</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>is_leaf_direct_parent</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>is_orphanet_disorder</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>is_omim</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>is_icd_category</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>is_icd_chapter_code</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>is_icd_chapter_header</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>is_icd_billable</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>is_mondo_subtype</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>is_pathway_defect</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>is_susceptibility</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>is_paraphilic</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>is_acquired</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>is_andor</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>is_withorwithout</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>is_obsoletion_candidate</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>is_unclassified_hereditary</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>official_matrix_filter</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>harrisons_view</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>mondo_txgnn</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>mondo_top_grouping</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>medical_specialization</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>txgnn</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>anatomical</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>is_pathogen_caused</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>is_cancer</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>is_glucose_dysfunction</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>tag_existing_treatment</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>tag_qaly_lost</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>subset_group_id</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>subset_group_label</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>other_subsets_count</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>disease_list_entries</t>
         </is>
       </c>

</xml_diff>